<commit_message>
Correction of the second test case
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\fmh_android_10_11_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83136792-1746-42A7-98FA-5B67F914CD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43B69A-3909-4F06-9C2C-C2F21AED771A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,6 +460,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -469,8 +472,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -480,9 +483,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B19" sqref="B19:D19"/>
     </sheetView>
   </sheetViews>
@@ -802,581 +802,624 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="122.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="8" t="s">
+      <c r="B58" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B59" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B42:D42"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
     <mergeCell ref="B59:D59"/>
@@ -1393,49 +1436,6 @@
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correction of the third test case
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\fmh_android_10_11_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43B69A-3909-4F06-9C2C-C2F21AED771A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFA21B6-A13F-4D5B-A66F-936DA2D68567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
   <si>
     <r>
       <rPr>
@@ -96,114 +96,6 @@
     </r>
   </si>
   <si>
-    <t>Проверка "Поле авторизации “login”"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка "Поле авторизации “password”"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для несуществующей категории "Путешествие"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "Зарплата"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка "Числовое поле «Дата начальная»"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка "Числовое поле «Дата конечная»"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "День рождения"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "Объявления"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "Праздник"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "Массаж"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "Благодарность"</t>
-  </si>
-  <si>
-    <t>Проверка Фильтр новостей для существующей категории "Нужна помощь"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Поле “Категория”(Category)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Поле “Заголовок”(Title)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Поле “Дата публикации”(Publication date)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Поле “Время”(Time)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Поле “Описание”(Description)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Кнопка “Сохранить”(Save)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Кнопка “Отмена”(Cancel)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Кнопка из контрольной панели «Сортировка по дате, от большей даты к меньшей и от меньшей даты к большей»</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Кнопка “Удалить”(Delete)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Кнопка “Редактирование”(Editing)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка Кнопка «Раскрытие активного комментария» </t>
-  </si>
-  <si>
-    <t>Проверка Создание новости действующей категории "Зарплата"</t>
-  </si>
-  <si>
-    <t>Проверка Создание новости действующей категории "Объявление"</t>
-  </si>
-  <si>
-    <t>Проверка Создание новости действующей категории "День рождения"</t>
-  </si>
-  <si>
-    <t>Проверка Создание новости действующей категории "Профсоюз"</t>
-  </si>
-  <si>
-    <t>Проверка Создание новости несуществующей категории "Услуги"</t>
-  </si>
-  <si>
-    <t>Проверка Создание новости действующей категории "День рождения" свыше 8 -ми в очередном списке редактируемых новостей самой отдалённой даты</t>
-  </si>
-  <si>
-    <t>Проверка "Страница авторизации пользователя при "режиме затемнения" мобильного устройства. Хорошая видимость кнопок, текстов и вводимых символов"</t>
-  </si>
-  <si>
-    <t>Проверка "Страница "Новости" мобильного приложения "вхосписе". Хорошая видимость кнопок и текста на странице при использовании "режима затемнения" мобильного устройства"</t>
-  </si>
-  <si>
-    <t>Проверка "Главная страница мобильного приложения "вхосписе". Хорошая видимость кнопок и текста на странице при использовании "режима затемнения" мобильного устройства"</t>
-  </si>
-  <si>
-    <t>Проверка "Страница цитат с заголовком "Главное - жить любя" и раскрытия цитат мобильного приложения "вхосписе". Хорошая видимость кнопок и текста на странице при использовании "режима затемнения" мобильного устройства"</t>
-  </si>
-  <si>
-    <t>Проверка "Открытие ссылки "Ползовательское соглашение" приложения "Вхосписе" по адресу “https://vhospice.org/#/terms-of-use”"</t>
-  </si>
-  <si>
-    <t>Проверка "Открытие ссылки "Политика конфиденциальности" приложения "Вхосписе" по адресу “https://vhospice.org/#/privacy-policy/”"</t>
-  </si>
-  <si>
-    <t>Проверка "Раскрытие содержимого в кнопке из главного меню "форма бабочки" комментария из цитат “Главное - жить любя” - «1 - 8»"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">	</t>
     </r>
@@ -234,15 +126,6 @@
       </rPr>
       <t>Группа из контрольной панели “Фильтр новостей”(Filter news)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка "Поле “Категория”"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка "Кнопка “Фильтр”"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Проверка "Кнопка “Отмена”"</t>
   </si>
   <si>
     <r>
@@ -286,9 +169,6 @@
     <t>Проверка соответствия перевода названия группы из контрольной панели "Фильтр новостей" русскоязычной версии приложения и "Creating News" англоязычной версии приложения</t>
   </si>
   <si>
-    <t>Проверка Создание новости действующей категории "Зарплата" свыше 8 -ми в очередном списке редактируемых новостей ближайшей даты</t>
-  </si>
-  <si>
     <t>Проверка кнопки "Главная"</t>
   </si>
   <si>
@@ -313,7 +193,157 @@
     <t>Тестирование производительности</t>
   </si>
   <si>
-    <t>Проверка Фильтр новостей для существующей категории "Профсоюз"</t>
+    <t>Проверка: Фильтр новостей для существующей категории "Профсоюз"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Категория”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка кнопки “Фильтр”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка кнопки “Отмена”</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для несуществующей категории "Путешествие"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "Зарплата"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "День рождения"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "Объявления"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "Праздник"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "Массаж"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "Благодарность"</t>
+  </si>
+  <si>
+    <t>Проверка фильтра новостей для существующей категории "Нужна помощь"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Категория”(Category)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Заголовок”(Title)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Дата публикации”(Publication date)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Время”(Time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Описание”(Description)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Сохранить”(Save)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля “Отмена”(Cancel)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка кнопки из контрольной панели «Сортировка по дате, от большей даты к меньшей и от меньшей даты к большей»</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка кнопки “Удалить”(Delete)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка кнопки “Редактирование”(Editing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка кнопки «Раскрытие активного комментария» </t>
+  </si>
+  <si>
+    <t>Проверка создания новости действующей категории "Объявление"</t>
+  </si>
+  <si>
+    <t>Проверка создания новости действующей категории "День рождения"</t>
+  </si>
+  <si>
+    <t>Проверка создания новости действующей категории "Профсоюз"</t>
+  </si>
+  <si>
+    <t>Проверка создания новости несуществующей категории "Услуги"</t>
+  </si>
+  <si>
+    <t>Проверка создания новости действующей категории "Зарплата" свыше 8 -ми в очередном списке редактируемых новостей ближайшей даты</t>
+  </si>
+  <si>
+    <t>Проверка создания новости действующей категории "День рождения" свыше 8 -ми в очередном списке редактируемых новостей самой отдалённой даты</t>
+  </si>
+  <si>
+    <t>Проверка раскрытия содержимого в кнопке из главного меню "форма бабочки" комментария из цитат “Главное - жить любя” - «1 - 8»</t>
+  </si>
+  <si>
+    <t>Проверка открытия ссылки "Политика конфиденциальности" приложения "Вхосписе" по адресу “https://vhospice.org/#/privacy-policy/”</t>
+  </si>
+  <si>
+    <t>Проверка открытия ссылки "Ползовательское соглашение" приложения "Вхосписе" по адресу “https://vhospice.org/#/terms-of-use”</t>
+  </si>
+  <si>
+    <t>Проверка страницы цитат с заголовком "Главное - жить любя" и раскрытия цитат мобильного приложения "вхосписе". Хорошая видимость кнопок и текста на странице при использовании "режима затемнения" мобильного устройства</t>
+  </si>
+  <si>
+    <t>Проверка главной страницы мобильного приложения "вхосписе". Хорошая видимость кнопок и текста на странице при использовании "режима затемнения" мобильного устройства</t>
+  </si>
+  <si>
+    <t>Проверка страницы "Новости" мобильного приложения "вхосписе". Хорошая видимость кнопок и текста на странице при использовании "режима затемнения" мобильного устройства</t>
+  </si>
+  <si>
+    <t>Проверка страницы авторизации пользователя при "режиме затемнения" мобильного устройства. Хорошая видимость кнопок, текстов и вводимых символов</t>
+  </si>
+  <si>
+    <t>Проверка создания новости действующей категории "Зарплата"</t>
+  </si>
+  <si>
+    <t>Проверка поля авторизации “login”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка поля авторизации “password”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка числового поля “Дата начальная”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Проверка числового поля “Дата конечная”</t>
+  </si>
+  <si>
+    <t>Проверка обновления страницы на разных страницах приложения</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на главной странице приложения</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на главной странице при раскрытии кнопки "все новости"</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице редактируемых новостей при создании новости</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице редактируемых новостей</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице фильтра новостей</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице "Новости"</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице цитат с названием "Главное - жить любя"</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице "Авторизация пользователя"</t>
+  </si>
+  <si>
+    <t>Проверка функции обновления страницы на странице "О приложении"</t>
   </si>
 </sst>
 </file>
@@ -460,9 +490,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -472,9 +499,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -483,6 +507,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -802,583 +832,681 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="122.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="B3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="B15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
+      <c r="B19" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
+      <c r="B20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
+      <c r="B23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
+      <c r="B24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
+      <c r="B26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="B28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
     </row>
     <row r="31" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="B32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="B34" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
     </row>
     <row r="35" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="B35" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="B36" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="8"/>
+      <c r="B38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="8"/>
+      <c r="B39" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="8"/>
+      <c r="B40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
+      <c r="B41" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="8"/>
+      <c r="B42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="8"/>
+      <c r="B43" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="6"/>
+      <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="7"/>
     </row>
     <row r="46" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="8"/>
+      <c r="A47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
+      <c r="A48" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B48" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="8"/>
+      <c r="B50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
+      <c r="B51" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12"/>
-    </row>
-    <row r="53" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="8"/>
+      <c r="A52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="8"/>
+      <c r="A54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="6"/>
+      <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="8"/>
+      <c r="A55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="6"/>
+      <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+        <v>65</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" s="6"/>
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+    </row>
+    <row r="70" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
+  <mergeCells count="69">
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
@@ -1391,7 +1519,7 @@
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B63:D63"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
@@ -1404,7 +1532,7 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B66:D66"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
@@ -1412,18 +1540,18 @@
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B49:D49"/>
     <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B67:D67"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B40:D40"/>
@@ -1433,9 +1561,19 @@
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B62:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing the fourth test case
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\fmh_android_10_11_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFA21B6-A13F-4D5B-A66F-936DA2D68567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F123C05F-27A9-4D9C-A993-9AB418609E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="76">
   <si>
     <r>
       <rPr>
@@ -345,12 +345,27 @@
   <si>
     <t>Проверка функции обновления страницы на странице "О приложении"</t>
   </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -383,6 +398,13 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -410,7 +432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -457,29 +479,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -490,29 +496,50 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,695 +845,1065 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61:D61"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="127.77734375" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16" style="6" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="122.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="122.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="8" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="11" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="11"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="E11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="11"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="E12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="11"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="11"/>
-    </row>
-    <row r="14" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="E13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="E14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="E15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-    </row>
-    <row r="21" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-    </row>
-    <row r="24" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="11" t="s">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="E25" s="4"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="11" t="s">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="11" t="s">
+      <c r="E27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="13"/>
       <c r="D28" s="11"/>
-    </row>
-    <row r="29" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="11" t="s">
+      <c r="E28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="11"/>
-    </row>
-    <row r="30" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="11" t="s">
+      <c r="E29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="11"/>
-    </row>
-    <row r="31" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="11" t="s">
+      <c r="E30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" ht="42.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="11" t="s">
+      <c r="E31" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="42.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="11" t="s">
+      <c r="E32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="11" t="s">
+      <c r="E33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="11"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="11" t="s">
+      <c r="E34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="11"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="11" t="s">
+      <c r="E35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="11" t="s">
+      <c r="E36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="11"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="E37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="5" t="s">
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="5" t="s">
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="5" t="s">
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="6"/>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="46" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="11" t="s">
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-    </row>
-    <row r="47" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="5" t="s">
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="5" t="s">
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="7"/>
-    </row>
-    <row r="49" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="11" t="s">
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+    </row>
+    <row r="49" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="7"/>
-    </row>
-    <row r="51" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="5" t="s">
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="5" t="s">
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="8" t="s">
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="10"/>
-    </row>
-    <row r="54" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B54" s="5" t="s">
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+    </row>
+    <row r="53" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="5" t="s">
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="5" t="s">
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="7"/>
-    </row>
-    <row r="57" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="7"/>
-    </row>
-    <row r="58" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="5" t="s">
+      <c r="B57" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="5" t="s">
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="7"/>
-    </row>
-    <row r="60" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
-    </row>
-    <row r="61" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="5" t="s">
+      <c r="B60" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="7"/>
-    </row>
-    <row r="62" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="5" t="s">
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="7"/>
-    </row>
-    <row r="63" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="8" t="s">
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="10"/>
-    </row>
-    <row r="64" spans="1:4" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B64" s="5" t="s">
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="5" t="s">
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="5" t="s">
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="6"/>
-      <c r="D66" s="7"/>
-    </row>
-    <row r="67" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B67" s="11" t="s">
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+    </row>
+    <row r="66" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="11"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C67" s="13"/>
       <c r="D67" s="11"/>
-    </row>
-    <row r="68" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C68" s="11"/>
+      <c r="E67" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" s="13"/>
       <c r="D68" s="11"/>
-    </row>
-    <row r="69" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="11"/>
+      <c r="E68" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" s="13"/>
       <c r="D69" s="11"/>
-    </row>
-    <row r="70" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
+      <c r="E69" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="B63:D63"/>
     <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
@@ -1519,7 +1916,7 @@
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B62:D62"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B2:D2"/>
@@ -1532,7 +1929,7 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
@@ -1540,18 +1937,18 @@
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B37:D37"/>
     <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B47:D47"/>
     <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B67:D67"/>
     <mergeCell ref="B68:D68"/>
     <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B66:D66"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B40:D40"/>
@@ -1561,19 +1958,19 @@
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B49:D49"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B52:D52"/>
     <mergeCell ref="B53:D53"/>
     <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B59:D59"/>
     <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
     <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B62:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>